<commit_message>
Ficha de EPI finalizada
</commit_message>
<xml_diff>
--- a/FICHA DE EPI Atualizada 15.01.2024.xlsx
+++ b/FICHA DE EPI Atualizada 15.01.2024.xlsx
@@ -500,7 +500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -542,24 +542,21 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -602,20 +599,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -625,9 +610,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -656,13 +638,28 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -969,33 +966,33 @@
   <dimension ref="A1:Z655"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="B3" sqref="B3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="26" width="8.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" style="16" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.7109375" style="16" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="26" width="8.7109375" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="26"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="25"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -1016,15 +1013,15 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="48" customHeight="1">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="26"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="25"/>
       <c r="H2" s="2"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -1049,15 +1046,13 @@
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="27">
-        <v>141</v>
-      </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="28" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="26"/>
+      <c r="F3" s="25"/>
       <c r="G3" s="5" t="s">
         <v>4</v>
       </c>
@@ -1087,19 +1082,19 @@
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="29" t="s">
+      <c r="B4" s="26"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="29" t="s">
+      <c r="F4" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="29" t="s">
+      <c r="G4" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="29" t="s">
+      <c r="H4" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I4" s="3"/>
@@ -1125,13 +1120,13 @@
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
       <c r="I5" s="1"/>
       <c r="J5" s="7"/>
       <c r="K5" s="1"/>
@@ -1155,13 +1150,13 @@
       <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -1185,13 +1180,13 @@
       <c r="A7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -1215,13 +1210,13 @@
       <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
       <c r="I8" s="1"/>
       <c r="J8" s="3"/>
       <c r="K8" s="1"/>
@@ -1242,14 +1237,14 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" ht="2.25" customHeight="1">
-      <c r="A9" s="37"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="40"/>
+      <c r="A9" s="49"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="52"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -1270,16 +1265,16 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="44"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="39"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -1300,16 +1295,16 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="42"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="44"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="39"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -1330,14 +1325,14 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A12" s="46"/>
-      <c r="B12" s="42"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="44"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="39"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -1358,14 +1353,14 @@
       <c r="Z12" s="3"/>
     </row>
     <row r="13" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A13" s="46"/>
-      <c r="B13" s="42"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="44"/>
+      <c r="A13" s="40"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="39"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -1386,16 +1381,16 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="42"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="44"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="39"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -1416,14 +1411,14 @@
       <c r="Z14" s="3"/>
     </row>
     <row r="15" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A15" s="46"/>
-      <c r="B15" s="42"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="44"/>
+      <c r="A15" s="40"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="39"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -1444,16 +1439,16 @@
       <c r="Z15" s="3"/>
     </row>
     <row r="16" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="42"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="44"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="39"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -1474,14 +1469,14 @@
       <c r="Z16" s="1"/>
     </row>
     <row r="17" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A17" s="46"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="44"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="39"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -1502,16 +1497,16 @@
       <c r="Z17" s="3"/>
     </row>
     <row r="18" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A18" s="45" t="s">
+      <c r="A18" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="42"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="44"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="39"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -1532,14 +1527,14 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A19" s="46"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="44"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="39"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -1560,16 +1555,16 @@
       <c r="Z19" s="3"/>
     </row>
     <row r="20" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="42"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
-      <c r="H20" s="44"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="39"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -1590,14 +1585,14 @@
       <c r="Z20" s="3"/>
     </row>
     <row r="21" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A21" s="46"/>
-      <c r="B21" s="42"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="44"/>
+      <c r="A21" s="40"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="39"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -1648,11 +1643,11 @@
       <c r="Z22" s="3"/>
     </row>
     <row r="23" spans="1:26" ht="26.25" customHeight="1">
-      <c r="A23" s="47"/>
-      <c r="B23" s="48"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
+      <c r="A23" s="41"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="11"/>
@@ -1676,16 +1671,16 @@
       <c r="Z23" s="3"/>
     </row>
     <row r="24" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A24" s="45" t="s">
+      <c r="A24" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="42"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="44"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="39"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -1706,14 +1701,14 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A25" s="50"/>
-      <c r="B25" s="51"/>
-      <c r="C25" s="52"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="52"/>
-      <c r="F25" s="52"/>
-      <c r="G25" s="52"/>
-      <c r="H25" s="53"/>
+      <c r="A25" s="44"/>
+      <c r="B25" s="45"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="47"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
@@ -1752,10 +1747,10 @@
       <c r="F26" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G26" s="54" t="s">
+      <c r="G26" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="H26" s="26"/>
+      <c r="H26" s="25"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
@@ -1775,15 +1770,15 @@
       <c r="Y26" s="3"/>
       <c r="Z26" s="3"/>
     </row>
-    <row r="27" spans="1:26" ht="20.25" customHeight="1">
-      <c r="A27" s="15"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
+    <row r="27" spans="1:26" ht="84" customHeight="1">
+      <c r="A27" s="18"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
       <c r="G27" s="55"/>
-      <c r="H27" s="26"/>
+      <c r="H27" s="25"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
@@ -1805,13 +1800,13 @@
     </row>
     <row r="28" spans="1:26" ht="18.75" customHeight="1">
       <c r="A28" s="3"/>
-      <c r="B28" s="20"/>
+      <c r="B28" s="15"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
-      <c r="G28" s="58"/>
-      <c r="H28" s="58"/>
+      <c r="G28" s="57"/>
+      <c r="H28" s="57"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
@@ -1833,13 +1828,13 @@
     </row>
     <row r="29" spans="1:26" ht="18.75" customHeight="1">
       <c r="A29" s="3"/>
-      <c r="B29" s="20"/>
+      <c r="B29" s="15"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="57"/>
-      <c r="H29" s="57"/>
+      <c r="G29" s="54"/>
+      <c r="H29" s="54"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
@@ -1861,13 +1856,13 @@
     </row>
     <row r="30" spans="1:26" ht="18.75" customHeight="1">
       <c r="A30" s="3"/>
-      <c r="B30" s="20"/>
+      <c r="B30" s="15"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
-      <c r="G30" s="57"/>
-      <c r="H30" s="57"/>
+      <c r="G30" s="54"/>
+      <c r="H30" s="54"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
@@ -1889,13 +1884,13 @@
     </row>
     <row r="31" spans="1:26" ht="18.75" customHeight="1">
       <c r="A31" s="3"/>
-      <c r="B31" s="20"/>
+      <c r="B31" s="15"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
-      <c r="G31" s="57"/>
-      <c r="H31" s="57"/>
+      <c r="G31" s="54"/>
+      <c r="H31" s="54"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
@@ -1917,13 +1912,13 @@
     </row>
     <row r="32" spans="1:26" ht="18.75" customHeight="1">
       <c r="A32" s="3"/>
-      <c r="B32" s="20"/>
+      <c r="B32" s="15"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="57"/>
-      <c r="H32" s="57"/>
+      <c r="G32" s="54"/>
+      <c r="H32" s="54"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
@@ -1945,13 +1940,13 @@
     </row>
     <row r="33" spans="1:26" ht="18.75" customHeight="1">
       <c r="A33" s="3"/>
-      <c r="B33" s="20"/>
+      <c r="B33" s="15"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
-      <c r="G33" s="57"/>
-      <c r="H33" s="57"/>
+      <c r="G33" s="54"/>
+      <c r="H33" s="54"/>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
@@ -1973,13 +1968,13 @@
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1">
       <c r="A34" s="3"/>
-      <c r="B34" s="20"/>
+      <c r="B34" s="15"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
-      <c r="G34" s="57"/>
-      <c r="H34" s="57"/>
+      <c r="G34" s="54"/>
+      <c r="H34" s="54"/>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
@@ -2001,13 +1996,13 @@
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1">
       <c r="A35" s="3"/>
-      <c r="B35" s="20"/>
+      <c r="B35" s="15"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
-      <c r="G35" s="57"/>
-      <c r="H35" s="57"/>
+      <c r="G35" s="54"/>
+      <c r="H35" s="54"/>
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
@@ -2029,13 +2024,13 @@
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1">
       <c r="A36" s="3"/>
-      <c r="B36" s="20"/>
+      <c r="B36" s="15"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
-      <c r="G36" s="57"/>
-      <c r="H36" s="57"/>
+      <c r="G36" s="54"/>
+      <c r="H36" s="54"/>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
@@ -2057,13 +2052,13 @@
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1">
       <c r="A37" s="3"/>
-      <c r="B37" s="20"/>
+      <c r="B37" s="15"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
-      <c r="G37" s="57"/>
-      <c r="H37" s="57"/>
+      <c r="G37" s="54"/>
+      <c r="H37" s="54"/>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
@@ -2085,13 +2080,13 @@
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1">
       <c r="A38" s="3"/>
-      <c r="B38" s="20"/>
+      <c r="B38" s="15"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
-      <c r="G38" s="57"/>
-      <c r="H38" s="57"/>
+      <c r="G38" s="54"/>
+      <c r="H38" s="54"/>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
@@ -2113,13 +2108,13 @@
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1">
       <c r="A39" s="3"/>
-      <c r="B39" s="20"/>
+      <c r="B39" s="15"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
-      <c r="G39" s="57"/>
-      <c r="H39" s="57"/>
+      <c r="G39" s="54"/>
+      <c r="H39" s="54"/>
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
@@ -2141,13 +2136,13 @@
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1">
       <c r="A40" s="3"/>
-      <c r="B40" s="20"/>
+      <c r="B40" s="15"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
-      <c r="G40" s="57"/>
-      <c r="H40" s="57"/>
+      <c r="G40" s="54"/>
+      <c r="H40" s="54"/>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
@@ -2169,13 +2164,13 @@
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1">
       <c r="A41" s="3"/>
-      <c r="B41" s="20"/>
+      <c r="B41" s="15"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
-      <c r="G41" s="57"/>
-      <c r="H41" s="57"/>
+      <c r="G41" s="54"/>
+      <c r="H41" s="54"/>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
@@ -2197,13 +2192,13 @@
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1">
       <c r="A42" s="3"/>
-      <c r="B42" s="20"/>
+      <c r="B42" s="15"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
-      <c r="G42" s="57"/>
-      <c r="H42" s="57"/>
+      <c r="G42" s="54"/>
+      <c r="H42" s="54"/>
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
@@ -2225,13 +2220,13 @@
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1">
       <c r="A43" s="3"/>
-      <c r="B43" s="20"/>
+      <c r="B43" s="15"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
-      <c r="G43" s="57"/>
-      <c r="H43" s="57"/>
+      <c r="G43" s="54"/>
+      <c r="H43" s="54"/>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
@@ -2253,13 +2248,13 @@
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1">
       <c r="A44" s="3"/>
-      <c r="B44" s="20"/>
+      <c r="B44" s="15"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
-      <c r="G44" s="57"/>
-      <c r="H44" s="57"/>
+      <c r="G44" s="54"/>
+      <c r="H44" s="54"/>
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
@@ -2281,13 +2276,13 @@
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1">
       <c r="A45" s="3"/>
-      <c r="B45" s="20"/>
+      <c r="B45" s="15"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
-      <c r="G45" s="57"/>
-      <c r="H45" s="57"/>
+      <c r="G45" s="54"/>
+      <c r="H45" s="54"/>
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
@@ -2309,13 +2304,13 @@
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1">
       <c r="A46" s="3"/>
-      <c r="B46" s="20"/>
+      <c r="B46" s="15"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
-      <c r="G46" s="57"/>
-      <c r="H46" s="57"/>
+      <c r="G46" s="54"/>
+      <c r="H46" s="54"/>
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
@@ -2337,13 +2332,13 @@
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1">
       <c r="A47" s="3"/>
-      <c r="B47" s="20"/>
+      <c r="B47" s="15"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
-      <c r="G47" s="57"/>
-      <c r="H47" s="57"/>
+      <c r="G47" s="54"/>
+      <c r="H47" s="54"/>
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
@@ -2365,13 +2360,13 @@
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1">
       <c r="A48" s="3"/>
-      <c r="B48" s="20"/>
+      <c r="B48" s="15"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
-      <c r="G48" s="57"/>
-      <c r="H48" s="57"/>
+      <c r="G48" s="54"/>
+      <c r="H48" s="54"/>
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>
       <c r="K48" s="3"/>
@@ -2393,13 +2388,13 @@
     </row>
     <row r="49" spans="1:26" ht="15.75" customHeight="1">
       <c r="A49" s="3"/>
-      <c r="B49" s="20"/>
+      <c r="B49" s="15"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
-      <c r="G49" s="57"/>
-      <c r="H49" s="57"/>
+      <c r="G49" s="54"/>
+      <c r="H49" s="54"/>
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
@@ -2421,13 +2416,13 @@
     </row>
     <row r="50" spans="1:26" ht="15.75" customHeight="1">
       <c r="A50" s="3"/>
-      <c r="B50" s="20"/>
+      <c r="B50" s="15"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
-      <c r="G50" s="57"/>
-      <c r="H50" s="57"/>
+      <c r="G50" s="54"/>
+      <c r="H50" s="54"/>
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
@@ -2449,13 +2444,13 @@
     </row>
     <row r="51" spans="1:26" ht="15.75" customHeight="1">
       <c r="A51" s="3"/>
-      <c r="B51" s="20"/>
+      <c r="B51" s="15"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
-      <c r="G51" s="57"/>
-      <c r="H51" s="57"/>
+      <c r="G51" s="54"/>
+      <c r="H51" s="54"/>
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
@@ -2477,13 +2472,13 @@
     </row>
     <row r="52" spans="1:26" ht="15.75" customHeight="1">
       <c r="A52" s="3"/>
-      <c r="B52" s="20"/>
+      <c r="B52" s="15"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
-      <c r="G52" s="57"/>
-      <c r="H52" s="57"/>
+      <c r="G52" s="54"/>
+      <c r="H52" s="54"/>
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
@@ -2505,13 +2500,13 @@
     </row>
     <row r="53" spans="1:26" ht="15.75" customHeight="1">
       <c r="A53" s="3"/>
-      <c r="B53" s="20"/>
+      <c r="B53" s="15"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
-      <c r="G53" s="57"/>
-      <c r="H53" s="57"/>
+      <c r="G53" s="54"/>
+      <c r="H53" s="54"/>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
@@ -2533,13 +2528,13 @@
     </row>
     <row r="54" spans="1:26" ht="15.75" customHeight="1">
       <c r="A54" s="3"/>
-      <c r="B54" s="20"/>
+      <c r="B54" s="15"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
-      <c r="G54" s="57"/>
-      <c r="H54" s="57"/>
+      <c r="G54" s="54"/>
+      <c r="H54" s="54"/>
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
@@ -2561,13 +2556,13 @@
     </row>
     <row r="55" spans="1:26" ht="15.75" customHeight="1">
       <c r="A55" s="3"/>
-      <c r="B55" s="20"/>
+      <c r="B55" s="15"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
-      <c r="G55" s="57"/>
-      <c r="H55" s="57"/>
+      <c r="G55" s="54"/>
+      <c r="H55" s="54"/>
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
@@ -2589,13 +2584,13 @@
     </row>
     <row r="56" spans="1:26" ht="15.75" customHeight="1">
       <c r="A56" s="3"/>
-      <c r="B56" s="20"/>
+      <c r="B56" s="15"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
-      <c r="G56" s="57"/>
-      <c r="H56" s="57"/>
+      <c r="G56" s="54"/>
+      <c r="H56" s="54"/>
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
@@ -2617,13 +2612,13 @@
     </row>
     <row r="57" spans="1:26" ht="15.75" customHeight="1">
       <c r="A57" s="3"/>
-      <c r="B57" s="20"/>
+      <c r="B57" s="15"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
-      <c r="G57" s="57"/>
-      <c r="H57" s="57"/>
+      <c r="G57" s="54"/>
+      <c r="H57" s="54"/>
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
@@ -2645,13 +2640,13 @@
     </row>
     <row r="58" spans="1:26" ht="15.75" customHeight="1">
       <c r="A58" s="3"/>
-      <c r="B58" s="20"/>
+      <c r="B58" s="15"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
-      <c r="G58" s="57"/>
-      <c r="H58" s="57"/>
+      <c r="G58" s="54"/>
+      <c r="H58" s="54"/>
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
@@ -2673,13 +2668,13 @@
     </row>
     <row r="59" spans="1:26" ht="15.75" customHeight="1">
       <c r="A59" s="3"/>
-      <c r="B59" s="20"/>
+      <c r="B59" s="15"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
-      <c r="G59" s="57"/>
-      <c r="H59" s="57"/>
+      <c r="G59" s="54"/>
+      <c r="H59" s="54"/>
       <c r="I59" s="3"/>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
@@ -2701,13 +2696,13 @@
     </row>
     <row r="60" spans="1:26" ht="15.75" customHeight="1">
       <c r="A60" s="3"/>
-      <c r="B60" s="20"/>
+      <c r="B60" s="15"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
-      <c r="G60" s="57"/>
-      <c r="H60" s="57"/>
+      <c r="G60" s="54"/>
+      <c r="H60" s="54"/>
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
@@ -2729,13 +2724,13 @@
     </row>
     <row r="61" spans="1:26" ht="15.75" customHeight="1">
       <c r="A61" s="3"/>
-      <c r="B61" s="20"/>
+      <c r="B61" s="15"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
-      <c r="G61" s="57"/>
-      <c r="H61" s="57"/>
+      <c r="G61" s="54"/>
+      <c r="H61" s="54"/>
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
@@ -2757,13 +2752,13 @@
     </row>
     <row r="62" spans="1:26" ht="15.75" customHeight="1">
       <c r="A62" s="3"/>
-      <c r="B62" s="20"/>
+      <c r="B62" s="15"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
-      <c r="G62" s="57"/>
-      <c r="H62" s="57"/>
+      <c r="G62" s="54"/>
+      <c r="H62" s="54"/>
       <c r="I62" s="3"/>
       <c r="J62" s="3"/>
       <c r="K62" s="3"/>
@@ -2785,13 +2780,13 @@
     </row>
     <row r="63" spans="1:26" ht="15.75" customHeight="1">
       <c r="A63" s="3"/>
-      <c r="B63" s="20"/>
+      <c r="B63" s="15"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
-      <c r="G63" s="57"/>
-      <c r="H63" s="57"/>
+      <c r="G63" s="54"/>
+      <c r="H63" s="54"/>
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
@@ -2813,13 +2808,13 @@
     </row>
     <row r="64" spans="1:26" ht="15.75" customHeight="1">
       <c r="A64" s="3"/>
-      <c r="B64" s="20"/>
+      <c r="B64" s="15"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
-      <c r="G64" s="57"/>
-      <c r="H64" s="57"/>
+      <c r="G64" s="54"/>
+      <c r="H64" s="54"/>
       <c r="I64" s="3"/>
       <c r="J64" s="3"/>
       <c r="K64" s="3"/>
@@ -2841,13 +2836,13 @@
     </row>
     <row r="65" spans="1:26" ht="15.75" customHeight="1">
       <c r="A65" s="3"/>
-      <c r="B65" s="20"/>
+      <c r="B65" s="15"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
-      <c r="G65" s="57"/>
-      <c r="H65" s="57"/>
+      <c r="G65" s="54"/>
+      <c r="H65" s="54"/>
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
@@ -2869,13 +2864,13 @@
     </row>
     <row r="66" spans="1:26" ht="15.75" customHeight="1">
       <c r="A66" s="3"/>
-      <c r="B66" s="20"/>
+      <c r="B66" s="15"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
-      <c r="G66" s="57"/>
-      <c r="H66" s="57"/>
+      <c r="G66" s="54"/>
+      <c r="H66" s="54"/>
       <c r="I66" s="3"/>
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
@@ -2897,13 +2892,13 @@
     </row>
     <row r="67" spans="1:26" ht="15.75" customHeight="1">
       <c r="A67" s="3"/>
-      <c r="B67" s="20"/>
+      <c r="B67" s="15"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
-      <c r="G67" s="57"/>
-      <c r="H67" s="57"/>
+      <c r="G67" s="54"/>
+      <c r="H67" s="54"/>
       <c r="I67" s="3"/>
       <c r="J67" s="3"/>
       <c r="K67" s="3"/>
@@ -2925,13 +2920,13 @@
     </row>
     <row r="68" spans="1:26" ht="15.75" customHeight="1">
       <c r="A68" s="3"/>
-      <c r="B68" s="20"/>
+      <c r="B68" s="15"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
-      <c r="G68" s="57"/>
-      <c r="H68" s="57"/>
+      <c r="G68" s="54"/>
+      <c r="H68" s="54"/>
       <c r="I68" s="3"/>
       <c r="J68" s="3"/>
       <c r="K68" s="3"/>
@@ -2953,13 +2948,13 @@
     </row>
     <row r="69" spans="1:26" ht="15.75" customHeight="1">
       <c r="A69" s="3"/>
-      <c r="B69" s="20"/>
+      <c r="B69" s="15"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
-      <c r="G69" s="57"/>
-      <c r="H69" s="57"/>
+      <c r="G69" s="54"/>
+      <c r="H69" s="54"/>
       <c r="I69" s="3"/>
       <c r="J69" s="3"/>
       <c r="K69" s="3"/>
@@ -2981,13 +2976,13 @@
     </row>
     <row r="70" spans="1:26" ht="15.75" customHeight="1">
       <c r="A70" s="3"/>
-      <c r="B70" s="20"/>
+      <c r="B70" s="15"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
-      <c r="G70" s="57"/>
-      <c r="H70" s="57"/>
+      <c r="G70" s="54"/>
+      <c r="H70" s="54"/>
       <c r="I70" s="3"/>
       <c r="J70" s="3"/>
       <c r="K70" s="3"/>
@@ -3009,13 +3004,13 @@
     </row>
     <row r="71" spans="1:26" ht="15.75" customHeight="1">
       <c r="A71" s="3"/>
-      <c r="B71" s="20"/>
+      <c r="B71" s="15"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
-      <c r="G71" s="57"/>
-      <c r="H71" s="57"/>
+      <c r="G71" s="54"/>
+      <c r="H71" s="54"/>
       <c r="I71" s="3"/>
       <c r="J71" s="3"/>
       <c r="K71" s="3"/>
@@ -3037,13 +3032,13 @@
     </row>
     <row r="72" spans="1:26" ht="15.75" customHeight="1">
       <c r="A72" s="3"/>
-      <c r="B72" s="20"/>
+      <c r="B72" s="15"/>
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
-      <c r="G72" s="57"/>
-      <c r="H72" s="57"/>
+      <c r="G72" s="54"/>
+      <c r="H72" s="54"/>
       <c r="I72" s="3"/>
       <c r="J72" s="3"/>
       <c r="K72" s="3"/>
@@ -3065,13 +3060,13 @@
     </row>
     <row r="73" spans="1:26" ht="15.75" customHeight="1">
       <c r="A73" s="3"/>
-      <c r="B73" s="20"/>
+      <c r="B73" s="15"/>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
-      <c r="G73" s="57"/>
-      <c r="H73" s="57"/>
+      <c r="G73" s="54"/>
+      <c r="H73" s="54"/>
       <c r="I73" s="3"/>
       <c r="J73" s="3"/>
       <c r="K73" s="3"/>
@@ -3093,13 +3088,13 @@
     </row>
     <row r="74" spans="1:26" ht="15.75" customHeight="1">
       <c r="A74" s="3"/>
-      <c r="B74" s="20"/>
+      <c r="B74" s="15"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
-      <c r="G74" s="57"/>
-      <c r="H74" s="57"/>
+      <c r="G74" s="54"/>
+      <c r="H74" s="54"/>
       <c r="I74" s="3"/>
       <c r="J74" s="3"/>
       <c r="K74" s="3"/>
@@ -3121,13 +3116,13 @@
     </row>
     <row r="75" spans="1:26" ht="15.75" customHeight="1">
       <c r="A75" s="3"/>
-      <c r="B75" s="20"/>
+      <c r="B75" s="15"/>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
       <c r="E75" s="3"/>
       <c r="F75" s="3"/>
-      <c r="G75" s="57"/>
-      <c r="H75" s="57"/>
+      <c r="G75" s="54"/>
+      <c r="H75" s="54"/>
       <c r="I75" s="3"/>
       <c r="J75" s="3"/>
       <c r="K75" s="3"/>
@@ -3149,13 +3144,13 @@
     </row>
     <row r="76" spans="1:26" ht="15.75" customHeight="1">
       <c r="A76" s="3"/>
-      <c r="B76" s="20"/>
+      <c r="B76" s="15"/>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
-      <c r="G76" s="57"/>
-      <c r="H76" s="57"/>
+      <c r="G76" s="54"/>
+      <c r="H76" s="54"/>
       <c r="I76" s="3"/>
       <c r="J76" s="3"/>
       <c r="K76" s="3"/>
@@ -3177,13 +3172,13 @@
     </row>
     <row r="77" spans="1:26" ht="15.75" customHeight="1">
       <c r="A77" s="3"/>
-      <c r="B77" s="20"/>
+      <c r="B77" s="15"/>
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
-      <c r="G77" s="57"/>
-      <c r="H77" s="57"/>
+      <c r="G77" s="54"/>
+      <c r="H77" s="54"/>
       <c r="I77" s="3"/>
       <c r="J77" s="3"/>
       <c r="K77" s="3"/>
@@ -3205,13 +3200,13 @@
     </row>
     <row r="78" spans="1:26" ht="15.75" customHeight="1">
       <c r="A78" s="3"/>
-      <c r="B78" s="20"/>
+      <c r="B78" s="15"/>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
-      <c r="G78" s="57"/>
-      <c r="H78" s="57"/>
+      <c r="G78" s="54"/>
+      <c r="H78" s="54"/>
       <c r="I78" s="3"/>
       <c r="J78" s="3"/>
       <c r="K78" s="3"/>
@@ -19361,7 +19356,7 @@
     </row>
     <row r="655" spans="1:26" ht="15.75" customHeight="1">
       <c r="A655" s="3"/>
-      <c r="B655" s="20"/>
+      <c r="B655" s="15"/>
       <c r="C655" s="3"/>
       <c r="D655" s="3"/>
       <c r="E655" s="3"/>
@@ -19802,7 +19797,6 @@
     <mergeCell ref="G90:H90"/>
     <mergeCell ref="G91:H91"/>
     <mergeCell ref="G92:H92"/>
-    <mergeCell ref="G83:H83"/>
     <mergeCell ref="G84:H84"/>
     <mergeCell ref="G85:H85"/>
     <mergeCell ref="G86:H86"/>
@@ -19812,8 +19806,7 @@
     <mergeCell ref="G76:H76"/>
     <mergeCell ref="G77:H77"/>
     <mergeCell ref="G78:H78"/>
-    <mergeCell ref="G69:H69"/>
-    <mergeCell ref="G70:H70"/>
+    <mergeCell ref="G82:H82"/>
     <mergeCell ref="G71:H71"/>
     <mergeCell ref="G72:H72"/>
     <mergeCell ref="G73:H73"/>
@@ -19822,9 +19815,7 @@
     <mergeCell ref="G66:H66"/>
     <mergeCell ref="G67:H67"/>
     <mergeCell ref="G68:H68"/>
-    <mergeCell ref="G59:H59"/>
-    <mergeCell ref="G60:H60"/>
-    <mergeCell ref="G61:H61"/>
+    <mergeCell ref="G83:H83"/>
     <mergeCell ref="G62:H62"/>
     <mergeCell ref="G63:H63"/>
     <mergeCell ref="G54:H54"/>
@@ -19832,16 +19823,17 @@
     <mergeCell ref="G56:H56"/>
     <mergeCell ref="G57:H57"/>
     <mergeCell ref="G58:H58"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="G69:H69"/>
+    <mergeCell ref="G70:H70"/>
     <mergeCell ref="G53:H53"/>
     <mergeCell ref="G44:H44"/>
     <mergeCell ref="G45:H45"/>
     <mergeCell ref="G46:H46"/>
     <mergeCell ref="G47:H47"/>
     <mergeCell ref="G48:H48"/>
+    <mergeCell ref="G59:H59"/>
+    <mergeCell ref="G60:H60"/>
+    <mergeCell ref="G61:H61"/>
     <mergeCell ref="G39:H39"/>
     <mergeCell ref="G40:H40"/>
     <mergeCell ref="G41:H41"/>
@@ -19851,7 +19843,6 @@
     <mergeCell ref="G79:H79"/>
     <mergeCell ref="G80:H80"/>
     <mergeCell ref="G81:H81"/>
-    <mergeCell ref="G82:H82"/>
     <mergeCell ref="G28:H28"/>
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="G30:H30"/>
@@ -19863,6 +19854,10 @@
     <mergeCell ref="G36:H36"/>
     <mergeCell ref="G37:H37"/>
     <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="G52:H52"/>
     <mergeCell ref="A18:H19"/>
     <mergeCell ref="A20:H21"/>
     <mergeCell ref="A23:E23"/>

</xml_diff>